<commit_message>
SUMTER case is deleted from the SC tool file. New version published into the orchestrator.
</commit_message>
<xml_diff>
--- a/STS IR Bot Performer/Data/Input/SC ST 389 tool.xlsx
+++ b/STS IR Bot Performer/Data/Input/SC ST 389 tool.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/STS IR Bot Performer/Data/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahuel.delacruz\OneDrive - Sovos Compliance\Desktop\Nahuel\Projects\STS Internal Review bot\STS IR Bot Performer\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{4B815033-9A48-4B8D-BD9E-C1F8D9F2D0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4E1B1BA-C1CE-40A9-BB17-F46226C3C125}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25A03FE-628F-44E0-A5E5-06A0DF0D809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="226">
   <si>
     <t>LOCAL OPTION</t>
   </si>
@@ -707,9 +707,6 @@
   </si>
   <si>
     <t>SALUDA</t>
-  </si>
-  <si>
-    <t>SUMTER</t>
   </si>
   <si>
     <t>WILLIAMSBURG</t>
@@ -1605,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,12 +2387,12 @@
         <v>225</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="0"/>
-        <v>12035</v>
+        <f t="shared" ref="G27" si="1">H27*100</f>
+        <v>986.00000000000011</v>
       </c>
       <c r="H27" s="1">
-        <f>SUMIF($A$2:$A$160,"*Sumter County*",$C$2:$C$160)</f>
-        <v>120.35</v>
+        <f>SUMIF($A$2:$A$160,"*Williamsburg County*",$C$2:$C$160)</f>
+        <v>9.8600000000000012</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="1"/>
@@ -2415,17 +2412,9 @@
         <f>detail!J32</f>
         <v>33.03</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="G28" s="1">
-        <f t="shared" si="0"/>
-        <v>986.00000000000011</v>
-      </c>
-      <c r="H28" s="1">
-        <f>SUMIF($A$2:$A$160,"*Williamsburg County*",$C$2:$C$160)</f>
-        <v>9.8600000000000012</v>
-      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
       <c r="I28" s="2"/>
       <c r="J28" s="1"/>
       <c r="K28" s="4"/>

</xml_diff>